<commit_message>
Save segment validation scenario description for markdown insertion
Adds concept of descriptive vs ID name for validation scenarios
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/AutomatedValidationTemplate.xlsx
+++ b/data/human/adult/validation/Scenarios/AutomatedValidationTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Patient" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,15 +22,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="92">
   <si>
     <t xml:space="preserve">Scenario Name</t>
   </si>
   <si>
+    <t xml:space="preserve">Scenario Identifier</t>
+  </si>
+  <si>
     <t xml:space="preserve">Patient File</t>
   </si>
   <si>
     <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descriptive Name Example 1</t>
   </si>
   <si>
     <t xml:space="preserve">Example1</t>
@@ -244,6 +250,9 @@
   </si>
   <si>
     <t xml:space="preserve">State File</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descriptive Name Example 2</t>
   </si>
   <si>
     <t xml:space="preserve">Example2</t>
@@ -308,7 +317,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -347,12 +356,25 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <u val="single"/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -668,11 +690,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -685,11 +707,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -697,7 +723,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -801,10 +827,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -929,7 +951,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1025,8 +1051,8 @@
   </sheetPr>
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1053,163 +1079,167 @@
         <v>1</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" s="12" customFormat="true" ht="74" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="n">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" s="13" customFormat="true" ht="74" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="11"/>
-    </row>
-    <row r="5" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
+      <c r="B4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="H4" s="12"/>
+    </row>
+    <row r="5" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="B5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="17"/>
+      <c r="C5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="18"/>
       <c r="G5" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" s="12" customFormat="true" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="19" t="s">
+    <row r="6" s="13" customFormat="true" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="22" t="s">
+      <c r="B6" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="22"/>
-    </row>
-    <row r="7" s="12" customFormat="true" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="23"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="26" t="s">
+      <c r="C6" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="26"/>
-    </row>
-    <row r="8" s="12" customFormat="true" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="23"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="26" t="s">
+      <c r="D6" s="21"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="26"/>
-    </row>
-    <row r="9" s="12" customFormat="true" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="23"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="26" t="s">
+      <c r="H6" s="23"/>
+    </row>
+    <row r="7" s="13" customFormat="true" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="26"/>
-    </row>
-    <row r="10" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-    </row>
-    <row r="11" s="12" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="32" t="s">
-        <v>6</v>
+      <c r="H7" s="27"/>
+    </row>
+    <row r="8" s="13" customFormat="true" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="24"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="27"/>
+    </row>
+    <row r="9" s="13" customFormat="true" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="24"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="27"/>
+    </row>
+    <row r="10" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+    </row>
+    <row r="11" s="13" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C11" s="33"/>
       <c r="D11" s="33"/>
       <c r="E11" s="33"/>
       <c r="F11" s="33"/>
-      <c r="G11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>9</v>
+      <c r="G11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="I11" s="34"/>
       <c r="J11" s="34"/>
@@ -1220,40 +1250,40 @@
       <c r="A12" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="10"/>
+      <c r="B12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
       <c r="H12" s="36"/>
     </row>
-    <row r="13" s="12" customFormat="true" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" s="13" customFormat="true" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E13" s="39" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F13" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>9</v>
+        <v>30</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="I13" s="34"/>
       <c r="J13" s="34"/>
@@ -1262,436 +1292,436 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="40" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B14" s="41" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E14" s="42" t="n">
         <v>25</v>
       </c>
       <c r="F14" s="41" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G14" s="43"/>
       <c r="H14" s="44"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="45" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D15" s="46" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E15" s="42" t="n">
         <v>50</v>
       </c>
       <c r="F15" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G15" s="48"/>
       <c r="H15" s="44"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="45" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B16" s="46" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D16" s="46" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E16" s="42" t="n">
         <v>100</v>
       </c>
       <c r="F16" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G16" s="48"/>
       <c r="H16" s="44"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="45" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B17" s="46" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C17" s="46" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E17" s="42" t="n">
         <v>15</v>
       </c>
       <c r="F17" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G17" s="48"/>
       <c r="H17" s="44"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="46" t="s">
-        <v>39</v>
-      </c>
       <c r="D18" s="46" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E18" s="42" t="n">
         <v>0</v>
       </c>
       <c r="F18" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G18" s="48"/>
       <c r="H18" s="44"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="45" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B19" s="46" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D19" s="46" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E19" s="42" t="n">
         <v>0</v>
       </c>
       <c r="F19" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G19" s="48"/>
       <c r="H19" s="44"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="45" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D20" s="49" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E20" s="42" t="n">
         <v>0</v>
       </c>
       <c r="F20" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G20" s="48"/>
       <c r="H20" s="44"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="50" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C21" s="46" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D21" s="46" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E21" s="42" t="n">
         <v>0</v>
       </c>
       <c r="F21" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G21" s="48"/>
       <c r="H21" s="44"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="50" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C22" s="51" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D22" s="46" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E22" s="52" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F22" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G22" s="48"/>
       <c r="H22" s="44"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="51" t="s">
-        <v>50</v>
-      </c>
       <c r="C23" s="51" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D23" s="46" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E23" s="42"/>
       <c r="F23" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G23" s="48"/>
       <c r="H23" s="44"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="51" t="s">
-        <v>56</v>
-      </c>
       <c r="D24" s="46" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E24" s="42" t="n">
         <v>1</v>
       </c>
       <c r="F24" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G24" s="54"/>
       <c r="H24" s="44"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="53" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B25" s="51" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C25" s="51" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D25" s="46" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E25" s="42" t="n">
         <v>1</v>
       </c>
       <c r="F25" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G25" s="54"/>
       <c r="H25" s="44"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="51" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="49" t="s">
         <v>61</v>
-      </c>
-      <c r="B26" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="51" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="49" t="s">
-        <v>59</v>
       </c>
       <c r="E26" s="42" t="n">
         <v>1</v>
       </c>
       <c r="F26" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G26" s="54"/>
       <c r="H26" s="44"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="53" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B27" s="51" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C27" s="51" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D27" s="46" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E27" s="42" t="n">
         <v>1</v>
       </c>
       <c r="F27" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G27" s="54"/>
       <c r="H27" s="44"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="53" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B28" s="51" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C28" s="46" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D28" s="46" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E28" s="42" t="n">
         <v>1</v>
       </c>
       <c r="F28" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G28" s="54"/>
       <c r="H28" s="44"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="53" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B29" s="51" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C29" s="46" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D29" s="46" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E29" s="42" t="n">
         <v>1</v>
       </c>
       <c r="F29" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G29" s="54"/>
       <c r="H29" s="44"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="53" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B30" s="51" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C30" s="46" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D30" s="46" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E30" s="42" t="n">
         <v>1</v>
       </c>
       <c r="F30" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G30" s="54"/>
       <c r="H30" s="44"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="53" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B31" s="51" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C31" s="46" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D31" s="46" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E31" s="42" t="n">
         <v>1</v>
       </c>
       <c r="F31" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G31" s="54"/>
       <c r="H31" s="44"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="55" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B32" s="56" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C32" s="56" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D32" s="57" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E32" s="42" t="n">
         <v>1</v>
       </c>
       <c r="F32" s="58" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G32" s="54"/>
       <c r="H32" s="44"/>
     </row>
-    <row r="33" s="12" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="32" t="s">
-        <v>6</v>
+    <row r="33" s="13" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C33" s="33"/>
       <c r="D33" s="33"/>
       <c r="E33" s="33"/>
       <c r="F33" s="33"/>
-      <c r="G33" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>9</v>
+      <c r="G33" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="I33" s="34"/>
       <c r="J33" s="34"/>
@@ -1703,7 +1733,7 @@
         <v>2</v>
       </c>
       <c r="B34" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C34" s="60"/>
       <c r="D34" s="60"/>
@@ -1716,10 +1746,10 @@
   <mergeCells count="18">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="F1:H1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="F2:H2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="G5:H5"/>
@@ -1750,8 +1780,8 @@
   </sheetPr>
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1775,164 +1805,168 @@
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2" t="s">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="E1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="3"/>
+      <c r="A2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="4"/>
       <c r="C2" s="63" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D2" s="63"/>
       <c r="E2" s="64" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
+        <v>75</v>
+      </c>
+      <c r="F2" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" s="12" customFormat="true" ht="74" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="n">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" s="13" customFormat="true" ht="74" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="H4" s="11"/>
-    </row>
-    <row r="5" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="14" t="s">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="12"/>
+    </row>
+    <row r="5" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="B5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="17"/>
+      <c r="C5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="18"/>
       <c r="G5" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" s="12" customFormat="true" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="19" t="s">
+    <row r="6" s="13" customFormat="true" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="22" t="s">
+      <c r="B6" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="22"/>
-    </row>
-    <row r="7" s="12" customFormat="true" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="23"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="26" t="s">
+      <c r="C6" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="26"/>
-    </row>
-    <row r="8" s="12" customFormat="true" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="23"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="26" t="s">
+      <c r="D6" s="21"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="26"/>
-    </row>
-    <row r="9" s="12" customFormat="true" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="23"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="26" t="s">
+      <c r="H6" s="23"/>
+    </row>
+    <row r="7" s="13" customFormat="true" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="26"/>
-    </row>
-    <row r="10" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-    </row>
-    <row r="11" s="12" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="32" t="s">
-        <v>6</v>
+      <c r="H7" s="27"/>
+    </row>
+    <row r="8" s="13" customFormat="true" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="24"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="27"/>
+    </row>
+    <row r="9" s="13" customFormat="true" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="24"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="27"/>
+    </row>
+    <row r="10" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+    </row>
+    <row r="11" s="13" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C11" s="33"/>
       <c r="D11" s="33"/>
       <c r="E11" s="33"/>
       <c r="F11" s="33"/>
-      <c r="G11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>9</v>
+      <c r="G11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="I11" s="34"/>
       <c r="J11" s="34"/>
@@ -1943,40 +1977,40 @@
       <c r="A12" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="10"/>
+      <c r="B12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
       <c r="H12" s="36"/>
     </row>
-    <row r="13" s="12" customFormat="true" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" s="13" customFormat="true" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E13" s="39" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F13" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>9</v>
+        <v>30</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="I13" s="0"/>
       <c r="J13" s="34"/>
@@ -1985,22 +2019,22 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="40" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B14" s="41" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E14" s="42" t="n">
         <v>25</v>
       </c>
       <c r="F14" s="41" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G14" s="43"/>
       <c r="H14" s="44"/>
@@ -2008,22 +2042,22 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="45" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D15" s="46" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E15" s="42" t="n">
         <v>50</v>
       </c>
       <c r="F15" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G15" s="48"/>
       <c r="H15" s="44"/>
@@ -2031,22 +2065,22 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="45" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B16" s="46" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D16" s="46" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E16" s="42" t="n">
         <v>100</v>
       </c>
       <c r="F16" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G16" s="48"/>
       <c r="H16" s="44"/>
@@ -2054,22 +2088,22 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="45" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B17" s="46" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C17" s="46" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E17" s="42" t="n">
         <v>15</v>
       </c>
       <c r="F17" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G17" s="48"/>
       <c r="H17" s="44"/>
@@ -2077,22 +2111,22 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="46" t="s">
-        <v>39</v>
-      </c>
       <c r="D18" s="46" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E18" s="42" t="n">
         <v>0</v>
       </c>
       <c r="F18" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G18" s="48"/>
       <c r="H18" s="44"/>
@@ -2100,22 +2134,22 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="45" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B19" s="46" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D19" s="46" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E19" s="42" t="n">
         <v>0</v>
       </c>
       <c r="F19" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G19" s="48"/>
       <c r="H19" s="44"/>
@@ -2123,22 +2157,22 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="45" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D20" s="49" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E20" s="42" t="n">
         <v>0</v>
       </c>
       <c r="F20" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G20" s="48"/>
       <c r="H20" s="44"/>
@@ -2146,22 +2180,22 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="50" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C21" s="46" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D21" s="46" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E21" s="42" t="n">
         <v>0</v>
       </c>
       <c r="F21" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G21" s="48"/>
       <c r="H21" s="44"/>
@@ -2169,22 +2203,22 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="50" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C22" s="51" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D22" s="46" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E22" s="52" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F22" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G22" s="48"/>
       <c r="H22" s="44"/>
@@ -2192,20 +2226,20 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="51" t="s">
-        <v>50</v>
-      </c>
       <c r="C23" s="51" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D23" s="46" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E23" s="42"/>
       <c r="F23" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G23" s="48"/>
       <c r="H23" s="44"/>
@@ -2213,22 +2247,22 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="51" t="s">
-        <v>56</v>
-      </c>
       <c r="D24" s="46" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E24" s="42" t="n">
         <v>1</v>
       </c>
       <c r="F24" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G24" s="54"/>
       <c r="H24" s="44"/>
@@ -2236,22 +2270,22 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="53" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B25" s="51" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C25" s="51" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D25" s="46" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E25" s="42" t="n">
         <v>1</v>
       </c>
       <c r="F25" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G25" s="54"/>
       <c r="H25" s="44"/>
@@ -2259,22 +2293,22 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="51" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="49" t="s">
         <v>61</v>
-      </c>
-      <c r="B26" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="51" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="49" t="s">
-        <v>59</v>
       </c>
       <c r="E26" s="42" t="n">
         <v>1</v>
       </c>
       <c r="F26" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G26" s="54"/>
       <c r="H26" s="44"/>
@@ -2282,22 +2316,22 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="53" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B27" s="51" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C27" s="51" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D27" s="46" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E27" s="42" t="n">
         <v>1</v>
       </c>
       <c r="F27" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G27" s="54"/>
       <c r="H27" s="44"/>
@@ -2305,22 +2339,22 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="53" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B28" s="51" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C28" s="46" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D28" s="46" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E28" s="42" t="n">
         <v>1</v>
       </c>
       <c r="F28" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G28" s="54"/>
       <c r="H28" s="44"/>
@@ -2328,22 +2362,22 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="53" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B29" s="51" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C29" s="46" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D29" s="46" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E29" s="42" t="n">
         <v>1</v>
       </c>
       <c r="F29" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G29" s="54"/>
       <c r="H29" s="44"/>
@@ -2351,22 +2385,22 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="53" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B30" s="51" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C30" s="46" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D30" s="46" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E30" s="42" t="n">
         <v>1</v>
       </c>
       <c r="F30" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G30" s="54"/>
       <c r="H30" s="44"/>
@@ -2374,22 +2408,22 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="53" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B31" s="51" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C31" s="46" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D31" s="46" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E31" s="42" t="n">
         <v>1</v>
       </c>
       <c r="F31" s="47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G31" s="54"/>
       <c r="H31" s="44"/>
@@ -2397,43 +2431,43 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="55" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B32" s="56" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C32" s="56" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D32" s="57" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E32" s="42" t="n">
         <v>1</v>
       </c>
       <c r="F32" s="58" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G32" s="54"/>
       <c r="H32" s="44"/>
       <c r="I32" s="0"/>
     </row>
-    <row r="33" s="12" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="32" t="s">
-        <v>6</v>
+    <row r="33" s="13" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C33" s="33"/>
       <c r="D33" s="33"/>
       <c r="E33" s="33"/>
       <c r="F33" s="33"/>
-      <c r="G33" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>9</v>
+      <c r="G33" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="I33" s="0"/>
       <c r="J33" s="34"/>
@@ -2445,7 +2479,7 @@
         <v>2</v>
       </c>
       <c r="B34" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C34" s="60"/>
       <c r="D34" s="60"/>
@@ -2458,10 +2492,10 @@
   <mergeCells count="18">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="F1:H1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="F2:H2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="G5:H5"/>
@@ -2476,7 +2510,7 @@
     <mergeCell ref="B34:F34"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="StandardMale@0s.json"/>
+    <hyperlink ref="E2" r:id="rId1" display="StandardMale@0s.json"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2495,182 +2529,182 @@
   </sheetPr>
   <dimension ref="B2:E44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G52" activeCellId="0" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="65" t="s">
-        <v>74</v>
+      <c r="B2" s="66" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="66" t="s">
-        <v>75</v>
+      <c r="B3" s="67" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="66" t="s">
-        <v>76</v>
+      <c r="B4" s="67" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="66" t="s">
-        <v>77</v>
+      <c r="B5" s="67" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="66" t="s">
-        <v>78</v>
+      <c r="B6" s="67" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="66" t="s">
-        <v>79</v>
+      <c r="C7" s="67" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="66" t="s">
-        <v>80</v>
+      <c r="C8" s="67" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="66" t="s">
-        <v>81</v>
+      <c r="B9" s="67" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="66" t="s">
-        <v>82</v>
+      <c r="B10" s="67" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="66" t="s">
-        <v>83</v>
+      <c r="C11" s="67" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="66" t="s">
-        <v>84</v>
+      <c r="C12" s="67" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="66" t="s">
-        <v>85</v>
+      <c r="C13" s="67" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="66" t="s">
-        <v>86</v>
+      <c r="C14" s="67" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="65" t="s">
-        <v>87</v>
+      <c r="B19" s="66" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="66" t="s">
-        <v>88</v>
+      <c r="B20" s="67" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="67"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="67"/>
+      <c r="B29" s="68"/>
+      <c r="C29" s="68"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="67"/>
-      <c r="C30" s="67"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
+      <c r="B30" s="68"/>
+      <c r="C30" s="68"/>
+      <c r="D30" s="68"/>
+      <c r="E30" s="68"/>
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="67"/>
-      <c r="C31" s="67"/>
-      <c r="D31" s="67"/>
-      <c r="E31" s="67"/>
+      <c r="B31" s="68"/>
+      <c r="C31" s="68"/>
+      <c r="D31" s="68"/>
+      <c r="E31" s="68"/>
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="67"/>
-      <c r="C32" s="67"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="67"/>
+      <c r="B32" s="68"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="68"/>
+      <c r="E32" s="68"/>
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="67"/>
-      <c r="C33" s="67"/>
-      <c r="D33" s="67"/>
-      <c r="E33" s="67"/>
+      <c r="B33" s="68"/>
+      <c r="C33" s="68"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="68"/>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="67"/>
-      <c r="C34" s="67"/>
-      <c r="D34" s="67"/>
-      <c r="E34" s="67"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="68"/>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="67"/>
-      <c r="C35" s="67"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="67"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="68"/>
+      <c r="D35" s="68"/>
+      <c r="E35" s="68"/>
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="67"/>
-      <c r="C36" s="67"/>
-      <c r="D36" s="67"/>
-      <c r="E36" s="67"/>
+      <c r="B36" s="68"/>
+      <c r="C36" s="68"/>
+      <c r="D36" s="68"/>
+      <c r="E36" s="68"/>
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="67"/>
-      <c r="C37" s="67"/>
-      <c r="D37" s="67"/>
-      <c r="E37" s="67"/>
+      <c r="B37" s="68"/>
+      <c r="C37" s="68"/>
+      <c r="D37" s="68"/>
+      <c r="E37" s="68"/>
     </row>
     <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="67"/>
-      <c r="C38" s="67"/>
-      <c r="D38" s="67"/>
-      <c r="E38" s="67"/>
+      <c r="B38" s="68"/>
+      <c r="C38" s="68"/>
+      <c r="D38" s="68"/>
+      <c r="E38" s="68"/>
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="67"/>
-      <c r="C39" s="67"/>
-      <c r="D39" s="67"/>
-      <c r="E39" s="67"/>
+      <c r="B39" s="68"/>
+      <c r="C39" s="68"/>
+      <c r="D39" s="68"/>
+      <c r="E39" s="68"/>
     </row>
     <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="67"/>
-      <c r="C40" s="67"/>
-      <c r="D40" s="67"/>
-      <c r="E40" s="67"/>
+      <c r="B40" s="68"/>
+      <c r="C40" s="68"/>
+      <c r="D40" s="68"/>
+      <c r="E40" s="68"/>
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="67"/>
-      <c r="C41" s="67"/>
-      <c r="D41" s="67"/>
-      <c r="E41" s="67"/>
+      <c r="B41" s="68"/>
+      <c r="C41" s="68"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="68"/>
     </row>
     <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="67"/>
-      <c r="C42" s="67"/>
-      <c r="D42" s="67"/>
-      <c r="E42" s="67"/>
+      <c r="B42" s="68"/>
+      <c r="C42" s="68"/>
+      <c r="D42" s="68"/>
+      <c r="E42" s="68"/>
     </row>
     <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="67"/>
-      <c r="C43" s="67"/>
-      <c r="D43" s="67"/>
-      <c r="E43" s="67"/>
+      <c r="B43" s="68"/>
+      <c r="C43" s="68"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="68"/>
     </row>
     <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="67"/>
-      <c r="C44" s="67"/>
-      <c r="D44" s="67"/>
-      <c r="E44" s="67"/>
+      <c r="B44" s="68"/>
+      <c r="C44" s="68"/>
+      <c r="D44" s="68"/>
+      <c r="E44" s="68"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>